<commit_message>
saving files for the weekend. Made updates to new bot
</commit_message>
<xml_diff>
--- a/bot/log.xlsx
+++ b/bot/log.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Logs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Filtered Logs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Filtered logs" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,27 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1"/>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,327 +426,39 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>hvcaeo</t>
+          <t>m8qyl7</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/whales/comments/hvcaeo/petition_to_protect_southern_resident_killer/</t>
+          <t>https://www.popsci.com/story/animals/sperm-whale-culture/</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Petition to Protect Southern Resident Killer Whales</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>kkjyn8</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://english.kyodonews.net/news/2020/12/f6eec6b85d4f-japan-sets-whaling-catch-limit-for-2021-at-383-same-as-2020.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Japan sets whaling catch limit for 2021 at 383, same as 2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>kjyqp5</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/u87xsvpu0c761.jpg</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Found these in my stocking this morning, I love the first one lol</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>kjl7d3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://v.redd.it/8nx7ux2lp4761</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Beautiful pod filmed by an angler!</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>kjus04</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://www.nytimes.com/2020/12/23/science/blue-whales-indian-ocean.html</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>A New Population of Blue Whales Was Discovered Hiding in the Indian Ocean</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>kjpmfi</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://www.local10.com/news/local/2020/12/24/protesters-gather-in-front-of-seaquarium-in-continued-quest-to-free-whale/?fbclid=IwAR1DCL0uIGh5quBxFTuGC3YeceB23_KymezvBKHQ5j8W3HscTV0pJpyGhKo</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Protesters gather in front of Seaquarium in continued quest to free whale</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>kj5lqv</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.independent.co.uk/news/science/blue-whale-population-indian-ocean-b1777606.html</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Previously unknown population of blue whales found living in Indian Ocean</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>kira55</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://v.redd.it/v3dtaiz42s661</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Big bois</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>kj4sj6</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=FsAfZxyw3r0</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>How Killer Whales are Changing the Arctic</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>hvcaeo</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/whales/comments/hvcaeo/petition_to_protect_southern_resident_killer/</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Petition to Protect Southern Resident Killer Whales</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>kkjyn8</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://english.kyodonews.net/news/2020/12/f6eec6b85d4f-japan-sets-whaling-catch-limit-for-2021-at-383-same-as-2020.html</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Japan sets whaling catch limit for 2021 at 383, same as 2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>kjyqp5</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/u87xsvpu0c761.jpg</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Found these in my stocking this morning, I love the first one lol</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>kjl7d3</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://v.redd.it/8nx7ux2lp4761</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Beautiful pod filmed by an angler!</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>kjus04</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://www.nytimes.com/2020/12/23/science/blue-whales-indian-ocean.html</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>A New Population of Blue Whales Was Discovered Hiding in the Indian Ocean</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>kjpmfi</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://www.local10.com/news/local/2020/12/24/protesters-gather-in-front-of-seaquarium-in-continued-quest-to-free-whale/?fbclid=IwAR1DCL0uIGh5quBxFTuGC3YeceB23_KymezvBKHQ5j8W3HscTV0pJpyGhKo</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Protesters gather in front of Seaquarium in continued quest to free whale</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>kj5lqv</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://www.independent.co.uk/news/science/blue-whale-population-indian-ocean-b1777606.html</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Previously unknown population of blue whales found living in Indian Ocean</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>kira55</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://v.redd.it/v3dtaiz42s661</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Big bois</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>kj4sj6</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=FsAfZxyw3r0</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>How Killer Whales are Changing the Arctic</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>kis2sj</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://v.redd.it/9aemekrk5u661</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Beautiful</t>
+          <t>Sperm whale culture is surprising deep—and useful</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>